<commit_message>
Implementado Telas na Planilha do Modelo de Negocio
</commit_message>
<xml_diff>
--- a/modelo_negocio.xlsx
+++ b/modelo_negocio.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\18 - DEPARTAMENTO DE PROJETOS\Elder\Importador\Conv-Dados\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="8595" windowHeight="4695" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="8595" windowHeight="4695" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Tela 1 - Layouts Por Empresa" sheetId="1" r:id="rId1"/>
     <sheet name="Tela 2 - Definição do Layout" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="Tela 3 - Configuração do Layout" sheetId="3" r:id="rId3"/>
+    <sheet name="Tela 4 - Conf. Campos Layout" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>TESTE 123</t>
   </si>
@@ -39,26 +45,86 @@
     <t>1 - Sistema Profit - Contas a Pagar e Receber</t>
   </si>
   <si>
-    <t>Nome:</t>
-  </si>
-  <si>
     <t>Tipo:</t>
   </si>
   <si>
-    <t>Contas a Pagar e Receber</t>
-  </si>
-  <si>
     <t>Separador de Campos:</t>
   </si>
   <si>
     <t>|</t>
+  </si>
+  <si>
+    <t>Campos Principais</t>
+  </si>
+  <si>
+    <t>Nota/Documento</t>
+  </si>
+  <si>
+    <t>Nome Campo</t>
+  </si>
+  <si>
+    <t>Configurar</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>Nome Fornecedor/Cliente</t>
+  </si>
+  <si>
+    <t>CNPJ Fornecedor/Cliente</t>
+  </si>
+  <si>
+    <t>Data Baixa</t>
+  </si>
+  <si>
+    <t>Data Vencimento</t>
+  </si>
+  <si>
+    <t>Data Emissão Nota</t>
+  </si>
+  <si>
+    <t>Valor Pago</t>
+  </si>
+  <si>
+    <t>Valor Recebido</t>
+  </si>
+  <si>
+    <t>Valor Juros</t>
+  </si>
+  <si>
+    <t>Valor Multa</t>
+  </si>
+  <si>
+    <t>Valor Desconto</t>
+  </si>
+  <si>
+    <t>Histórico</t>
+  </si>
+  <si>
+    <t>Campos Adicionais</t>
+  </si>
+  <si>
+    <t>Tipo Pagamento</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Plano de Contas</t>
+  </si>
+  <si>
+    <t>Empresa</t>
+  </si>
+  <si>
+    <t>Campo:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +148,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -91,7 +197,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -99,77 +205,51 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -179,6 +259,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -433,7 +516,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -468,7 +551,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -677,10 +760,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="B1" sqref="B1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,137 +771,181 @@
     <col min="1" max="1" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="9"/>
+      <c r="B3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="4">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="4">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="8"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="9"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="P8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="9"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="C4:K4"/>
+    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
     <mergeCell ref="C7:K7"/>
     <mergeCell ref="C8:K8"/>
     <mergeCell ref="C9:K9"/>
     <mergeCell ref="C10:K10"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="C4:K4"/>
-    <mergeCell ref="C5:K5"/>
-    <mergeCell ref="C6:K6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -828,75 +955,331 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="18"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="18"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="18"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:H1"/>
-    <mergeCell ref="C3:I3"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B3:I3"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
@@ -909,12 +1292,226 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="32.7109375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B18:D18"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:H1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implementado parte das Regras no Modelo de Negocio
</commit_message>
<xml_diff>
--- a/modelo_negocio.xlsx
+++ b/modelo_negocio.xlsx
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="77">
   <si>
     <t>TESTE 123</t>
   </si>
@@ -278,13 +278,43 @@
   </si>
   <si>
     <t>BAIXA</t>
+  </si>
+  <si>
+    <t>Regra:</t>
+  </si>
+  <si>
+    <t>Campo Conta Débito</t>
+  </si>
+  <si>
+    <t>Nome:</t>
+  </si>
+  <si>
+    <t>Retorna conta débito</t>
+  </si>
+  <si>
+    <t>Tipo Retorno:</t>
+  </si>
+  <si>
+    <t>Busca Dados da Domínio</t>
+  </si>
+  <si>
+    <t>1º Grupo de Condições:</t>
+  </si>
+  <si>
+    <t>1º comparação:</t>
+  </si>
+  <si>
+    <t>IGUAL AO</t>
+  </si>
+  <si>
+    <t>CNPJ Fornecedor (Busca do Fiscal na Domínio)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,6 +415,29 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -496,7 +549,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -513,14 +566,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -536,38 +585,18 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -579,9 +608,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -590,23 +616,14 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -614,20 +631,65 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1362,162 +1424,162 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
       <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
       <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
-      <c r="B3" s="31" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
       <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
-      <c r="B4" s="34">
+      <c r="A4" s="25"/>
+      <c r="B4" s="28">
         <v>1</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
+      <c r="D4" s="55"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
+      <c r="I4" s="55"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="55"/>
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-      <c r="B5" s="34">
+      <c r="A5" s="25"/>
+      <c r="B5" s="28">
         <v>2</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
-      <c r="B6" s="34"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="55"/>
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="55"/>
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
+      <c r="A8" s="25"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="55"/>
       <c r="L8" s="9"/>
       <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="55"/>
+      <c r="K10" s="55"/>
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -1531,7 +1593,7 @@
       <c r="L11" s="9"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -1545,7 +1607,7 @@
       <c r="L12" s="9"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -1559,7 +1621,7 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -1573,7 +1635,7 @@
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1587,7 +1649,7 @@
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1700,6 +1762,9 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
     <mergeCell ref="C7:K7"/>
     <mergeCell ref="C8:K8"/>
     <mergeCell ref="C9:K9"/>
@@ -1707,9 +1772,6 @@
     <mergeCell ref="C4:K4"/>
     <mergeCell ref="C5:K5"/>
     <mergeCell ref="C6:K6"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1733,351 +1795,351 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="52" t="s">
+      <c r="B1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="40"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
       <c r="M2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
-      <c r="L3" s="53"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="44"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="56"/>
-      <c r="B4" s="59"/>
-      <c r="C4" s="59"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="59"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
+      <c r="A4" s="43"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
       <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="60" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="62"/>
-      <c r="H5" s="62"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="53"/>
-      <c r="K5" s="53"/>
-      <c r="L5" s="53"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="61"/>
+      <c r="I5" s="61"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
       <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="53"/>
-      <c r="B6" s="53"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="53"/>
-      <c r="F6" s="53"/>
-      <c r="G6" s="53"/>
-      <c r="H6" s="53"/>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
-      <c r="L6" s="53"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
       <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="53"/>
-      <c r="B7" s="63" t="s">
+      <c r="A7" s="40"/>
+      <c r="B7" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64" t="s">
+      <c r="C7" s="59"/>
+      <c r="D7" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="53"/>
-      <c r="F7" s="53"/>
-      <c r="G7" s="53"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="53"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
       <c r="M7" s="1"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="53"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="53"/>
-      <c r="F8" s="53"/>
-      <c r="G8" s="53"/>
-      <c r="H8" s="53"/>
-      <c r="I8" s="53"/>
-      <c r="J8" s="53"/>
-      <c r="K8" s="53"/>
-      <c r="L8" s="53"/>
+      <c r="A8" s="40"/>
+      <c r="B8" s="40"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
       <c r="M8" s="1"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="53"/>
-      <c r="B9" s="63" t="s">
+      <c r="A9" s="40"/>
+      <c r="B9" s="59" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="63"/>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="54" t="s">
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="53"/>
-      <c r="J9" s="53"/>
-      <c r="K9" s="53"/>
-      <c r="L9" s="53"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
       <c r="M9" s="1"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="53"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
+      <c r="A10" s="40"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
       <c r="M10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="53"/>
-      <c r="B11" s="63" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="63"/>
-      <c r="J11" s="61" t="s">
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="60" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
       <c r="M11" s="1"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
-      <c r="C12" s="54"/>
-      <c r="D12" s="55"/>
-      <c r="E12" s="53"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="53"/>
-      <c r="K12" s="53"/>
-      <c r="L12" s="53"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
       <c r="M12" s="1"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="53"/>
-      <c r="B13" s="53"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
-      <c r="I13" s="53"/>
-      <c r="J13" s="53"/>
-      <c r="K13" s="53"/>
-      <c r="L13" s="53"/>
+      <c r="A13" s="40"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="53"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="53"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
+      <c r="A14" s="40"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
       <c r="M14" s="1"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="53"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="54"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="53"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="53"/>
-      <c r="I15" s="53"/>
-      <c r="J15" s="53"/>
-      <c r="K15" s="53"/>
-      <c r="L15" s="53"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="40"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
       <c r="M15" s="1"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="53"/>
-      <c r="B16" s="53"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="53"/>
-      <c r="F16" s="53"/>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="53"/>
-      <c r="K16" s="53"/>
-      <c r="L16" s="53"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
       <c r="M16" s="1"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="53"/>
-      <c r="B17" s="53"/>
-      <c r="C17" s="54"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
       <c r="M17" s="1"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="53"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
       <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="53"/>
-      <c r="B19" s="53"/>
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="53"/>
-      <c r="G19" s="53"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
       <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="48"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="48"/>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="48"/>
-      <c r="L20" s="48"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="48"/>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48"/>
-      <c r="K21" s="48"/>
-      <c r="L21" s="48"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="B3:F3"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="C5:I5"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:I5">
@@ -2099,7 +2161,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2114,303 +2176,303 @@
       <c r="A1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="15"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="16" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="16" t="s">
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="17" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="17" t="s">
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="16" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="19" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="24" t="s">
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="19" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="24" t="s">
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="20" t="s">
+      <c r="H6" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="19" t="s">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="24" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="20" t="s">
+      <c r="H7" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="21" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="20" t="s">
+      <c r="D8" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="24" t="s">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="20" t="s">
+      <c r="H8" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="22" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="24" t="s">
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="H9" s="20" t="s">
+      <c r="H9" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="22" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="24" t="s">
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="H10" s="20" t="s">
+      <c r="H10" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="23" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="20"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="18"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="23" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="20"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="18"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="19" t="s">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="20" t="s">
+      <c r="D13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="20"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="18"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="19" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="20"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="18"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="19" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="20"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="19" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="20"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="18"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="19" t="s">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="15"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="14"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="15"/>
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="14"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="15"/>
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="14"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="15"/>
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="14"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="15"/>
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2428,7 +2490,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15:N15"/>
+      <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,28 +2504,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="B1" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
       <c r="I1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
+      <c r="K1" s="76"/>
+      <c r="L1" s="76"/>
+      <c r="M1" s="76"/>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
@@ -2483,39 +2545,39 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="I3" s="9"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="66" t="s">
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="48" t="s">
         <v>55</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="9"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="69" t="s">
+      <c r="J4" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="66" t="s">
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="48" t="s">
         <v>41</v>
       </c>
       <c r="N4" s="6"/>
@@ -2523,69 +2585,69 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="68" t="s">
+      <c r="C5" s="69"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="66" t="s">
+      <c r="F5" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="50" t="s">
         <v>62</v>
       </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="65"/>
-      <c r="L5" s="65"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="66" t="s">
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="50"/>
+      <c r="N5" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="O5" s="68"/>
+      <c r="O5" s="50"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
-      <c r="B6" s="69" t="s">
+      <c r="B6" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="67" t="s">
+      <c r="C6" s="68"/>
+      <c r="D6" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="69" t="s">
+      <c r="J6" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="69"/>
-      <c r="L6" s="67" t="s">
+      <c r="K6" s="68"/>
+      <c r="L6" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="6"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
+      <c r="J7" s="67"/>
+      <c r="K7" s="67"/>
       <c r="L7" s="6"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -2593,26 +2655,26 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="44" t="s">
+      <c r="C8" s="67"/>
+      <c r="D8" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
       <c r="G8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="39" t="s">
+      <c r="J8" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="39"/>
-      <c r="L8" s="44" t="s">
+      <c r="K8" s="67"/>
+      <c r="L8" s="71" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="44"/>
-      <c r="N8" s="44"/>
+      <c r="M8" s="71"/>
+      <c r="N8" s="71"/>
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2633,53 +2695,53 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="74" t="s">
+      <c r="B10" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="75"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="70"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="51"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="74" t="s">
+      <c r="J10" s="72" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="75"/>
-      <c r="L10" s="40" t="s">
+      <c r="K10" s="73"/>
+      <c r="L10" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="M10" s="32"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="70"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="51"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="9"/>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="42">
+      <c r="C11" s="74"/>
+      <c r="D11" s="32">
         <v>4</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="32">
         <v>4</v>
       </c>
-      <c r="G11" s="70"/>
+      <c r="G11" s="51"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="41" t="s">
+      <c r="J11" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="K11" s="41"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42" t="s">
+      <c r="K11" s="74"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="N11" s="42"/>
-      <c r="O11" s="70"/>
+      <c r="N11" s="32"/>
+      <c r="O11" s="51"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="9"/>
@@ -2688,7 +2750,7 @@
       <c r="D12" s="6"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="70"/>
+      <c r="G12" s="51"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
@@ -2699,16 +2761,16 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="71"/>
-      <c r="D13" s="45" t="s">
+      <c r="C13" s="75"/>
+      <c r="D13" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="72"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="52"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
@@ -2719,72 +2781,72 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="30"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="30"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="43" t="s">
+      <c r="J14" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="K14" s="43"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="43"/>
-      <c r="N14" s="43"/>
+      <c r="K14" s="66"/>
+      <c r="L14" s="66"/>
+      <c r="M14" s="66"/>
+      <c r="N14" s="66"/>
       <c r="O14" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="73"/>
-      <c r="C15" s="73"/>
-      <c r="D15" s="45"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="67" t="s">
         <v>46</v>
       </c>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
+      <c r="K15" s="67"/>
+      <c r="L15" s="67"/>
+      <c r="M15" s="67"/>
+      <c r="N15" s="67"/>
       <c r="O15" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="71"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="46"/>
-      <c r="G16" s="30"/>
+      <c r="B16" s="75"/>
+      <c r="C16" s="75"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="26"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="39" t="s">
+      <c r="J16" s="67" t="s">
         <v>47</v>
       </c>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
+      <c r="K16" s="67"/>
+      <c r="L16" s="67"/>
+      <c r="M16" s="67"/>
+      <c r="N16" s="67"/>
       <c r="O16" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="26"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
@@ -2795,12 +2857,12 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
+      <c r="B18" s="75"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
@@ -2842,16 +2904,32 @@
       <c r="O20" s="9"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" s="36"/>
-      <c r="B21" s="37"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
+      <c r="A21" s="29"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="J14:N14"/>
     <mergeCell ref="J15:N15"/>
     <mergeCell ref="J16:N16"/>
@@ -2864,22 +2942,6 @@
     <mergeCell ref="L8:N8"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J11:K11"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 K3 L8:L9">
@@ -2906,7 +2968,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2915,15 +2977,15 @@
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
@@ -2943,15 +3005,15 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="78" t="s">
+      <c r="B3" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="78"/>
-      <c r="D3" s="33" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -2960,15 +3022,15 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="78"/>
-      <c r="D4" s="33" t="s">
+      <c r="C4" s="79"/>
+      <c r="D4" s="70" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="70"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -3216,12 +3278,142 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="81" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="82" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="81"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="83"/>
+      <c r="D5" s="80" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="84" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D9" s="85" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="86" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="87"/>
+      <c r="L9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="C8:E8"/>
+  </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5">
+      <formula1>"Busca Dados da Domínio,Agrupa Campos,Calcula Valor,Analisa Condições,Valor Fixo"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9:K9">
+      <formula1>"CONTÉM O VALOR,IGUAL AO,ENTRE,MAIOR QUE,MAIOR OU IGUAL À,MENOR QUE,MENOR OU IGUAL À"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9">
+      <formula1>"CNPJ Fornecedor (Busca do Fiscal na Domínio)"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'Tela 3 - Configuração do Layout'!$C$5:$C$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>E9</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Inicio da criacao do entities.models e feito algumas melhorias na planilha de Modego de Negocio
</commit_message>
<xml_diff>
--- a/modelo_negocio.xlsx
+++ b/modelo_negocio.xlsx
@@ -640,6 +640,9 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -648,9 +651,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -667,22 +667,22 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1427,48 +1427,48 @@
       <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
       <c r="L1" s="9"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="59"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
       <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="25"/>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
       <c r="L3" s="9"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1476,17 +1476,17 @@
       <c r="B4" s="28">
         <v>1</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="61"/>
-      <c r="J4" s="61"/>
-      <c r="K4" s="61"/>
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
       <c r="L4" s="9"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1494,88 +1494,88 @@
       <c r="B5" s="28">
         <v>2</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="58"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="58"/>
+      <c r="H5" s="58"/>
+      <c r="I5" s="58"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
       <c r="L5" s="9"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="28"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
+      <c r="C6" s="58"/>
+      <c r="D6" s="58"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
       <c r="L6" s="9"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="25"/>
       <c r="B7" s="28"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="61"/>
-      <c r="K7" s="61"/>
+      <c r="C7" s="58"/>
+      <c r="D7" s="58"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="58"/>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
       <c r="L7" s="9"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="25"/>
       <c r="B8" s="28"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="61"/>
-      <c r="J8" s="61"/>
-      <c r="K8" s="61"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="58"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="58"/>
       <c r="L8" s="9"/>
       <c r="P8" s="3"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="25"/>
       <c r="B9" s="28"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="58"/>
+      <c r="I9" s="58"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="58"/>
       <c r="L9" s="9"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="25"/>
       <c r="B10" s="28"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
       <c r="L10" s="9"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1762,16 +1762,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="C7:K7"/>
+    <mergeCell ref="C8:K8"/>
     <mergeCell ref="C9:K9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="C4:K4"/>
     <mergeCell ref="C5:K5"/>
     <mergeCell ref="C6:K6"/>
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="C7:K7"/>
-    <mergeCell ref="C8:K8"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2490,7 +2490,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D8" sqref="D8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2507,25 +2507,25 @@
       <c r="A1" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="71" t="s">
+      <c r="B1" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
       <c r="I1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="69" t="s">
+      <c r="J1" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
@@ -2546,37 +2546,37 @@
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
       <c r="B3" s="35"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
+      <c r="C3" s="80"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="80"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="35"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="80"/>
       <c r="N3" s="9"/>
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="74"/>
-      <c r="D4" s="74"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
       <c r="E4" s="48" t="s">
         <v>55</v>
       </c>
       <c r="F4" s="6"/>
       <c r="G4" s="9"/>
       <c r="I4" s="9"/>
-      <c r="J4" s="74" t="s">
+      <c r="J4" s="71" t="s">
         <v>56</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
+      <c r="K4" s="71"/>
+      <c r="L4" s="71"/>
       <c r="M4" s="48" t="s">
         <v>41</v>
       </c>
@@ -2585,11 +2585,11 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
       <c r="E5" s="50" t="s">
         <v>61</v>
       </c>
@@ -2600,11 +2600,11 @@
         <v>62</v>
       </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="75" t="s">
+      <c r="J5" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="K5" s="75"/>
-      <c r="L5" s="75"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
       <c r="M5" s="50"/>
       <c r="N5" s="48" t="s">
         <v>35</v>
@@ -2613,41 +2613,41 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="C6" s="74"/>
+      <c r="C6" s="71"/>
       <c r="D6" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="76" t="s">
+      <c r="E6" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="74" t="s">
+      <c r="J6" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="K6" s="74"/>
+      <c r="K6" s="71"/>
       <c r="L6" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="M6" s="76"/>
-      <c r="N6" s="76"/>
-      <c r="O6" s="76"/>
+      <c r="M6" s="73"/>
+      <c r="N6" s="73"/>
+      <c r="O6" s="73"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="6"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
       <c r="L7" s="6"/>
       <c r="M7" s="9"/>
       <c r="N7" s="9"/>
@@ -2655,26 +2655,26 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="72"/>
-      <c r="D8" s="80" t="s">
+      <c r="C8" s="70"/>
+      <c r="D8" s="74" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="80"/>
-      <c r="F8" s="80"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
       <c r="G8" s="9"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="72" t="s">
+      <c r="J8" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="72"/>
-      <c r="L8" s="80" t="s">
+      <c r="K8" s="70"/>
+      <c r="L8" s="74" t="s">
         <v>32</v>
       </c>
-      <c r="M8" s="80"/>
-      <c r="N8" s="80"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
       <c r="O8" s="9"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2695,19 +2695,19 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9"/>
-      <c r="B10" s="78" t="s">
+      <c r="B10" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="79"/>
+      <c r="C10" s="76"/>
       <c r="D10" s="31"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
       <c r="G10" s="51"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="78" t="s">
+      <c r="J10" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="79"/>
+      <c r="K10" s="76"/>
       <c r="L10" s="31" t="s">
         <v>40</v>
       </c>
@@ -2761,10 +2761,10 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="73" t="s">
+      <c r="B13" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="73"/>
+      <c r="C13" s="78"/>
       <c r="D13" s="33" t="s">
         <v>36</v>
       </c>
@@ -2788,13 +2788,13 @@
       <c r="F14" s="26"/>
       <c r="G14" s="26"/>
       <c r="I14" s="9"/>
-      <c r="J14" s="81" t="s">
+      <c r="J14" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="K14" s="81"/>
-      <c r="L14" s="81"/>
-      <c r="M14" s="81"/>
-      <c r="N14" s="81"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="69"/>
+      <c r="M14" s="69"/>
+      <c r="N14" s="69"/>
       <c r="O14" s="6" t="s">
         <v>41</v>
       </c>
@@ -2808,33 +2808,33 @@
       <c r="F15" s="26"/>
       <c r="G15" s="26"/>
       <c r="I15" s="9"/>
-      <c r="J15" s="72" t="s">
+      <c r="J15" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="72"/>
+      <c r="K15" s="70"/>
+      <c r="L15" s="70"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="70"/>
       <c r="O15" s="6" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="73"/>
+      <c r="B16" s="78"/>
+      <c r="C16" s="78"/>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
       <c r="F16" s="34"/>
       <c r="G16" s="26"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="72" t="s">
+      <c r="J16" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="72"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="70"/>
+      <c r="M16" s="70"/>
+      <c r="N16" s="70"/>
       <c r="O16" s="6" t="s">
         <v>48</v>
       </c>
@@ -2857,8 +2857,8 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="73"/>
-      <c r="C18" s="73"/>
+      <c r="B18" s="78"/>
+      <c r="C18" s="78"/>
       <c r="D18" s="33"/>
       <c r="E18" s="26"/>
       <c r="F18" s="26"/>
@@ -2914,6 +2914,22 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="J14:N14"/>
     <mergeCell ref="J15:N15"/>
     <mergeCell ref="J16:N16"/>
@@ -2926,22 +2942,6 @@
     <mergeCell ref="L8:N8"/>
     <mergeCell ref="J10:K10"/>
     <mergeCell ref="J11:K11"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="B7:C7"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D8:D9 K3 L8:L9">
@@ -2977,15 +2977,15 @@
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
       <c r="K1" s="9"/>
@@ -3009,11 +3009,11 @@
         <v>49</v>
       </c>
       <c r="C3" s="82"/>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
@@ -3026,11 +3026,11 @@
         <v>51</v>
       </c>
       <c r="C4" s="82"/>
-      <c r="D4" s="76" t="s">
+      <c r="D4" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
       <c r="I4" s="9"/>
@@ -3281,7 +3281,7 @@
   <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3290,15 +3290,15 @@
       <c r="A1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="79" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>

</xml_diff>